<commit_message>
Updating count numbers for under_ice_rerun projects
</commit_message>
<xml_diff>
--- a/scripts/projects/under_ice_rerun/meta_data.xlsx
+++ b/scripts/projects/under_ice_rerun/meta_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="327">
   <si>
     <t>Sample</t>
   </si>
@@ -862,6 +862,144 @@
   </si>
   <si>
     <t>v2.2.58</t>
+  </si>
+  <si>
+    <t>2f43253d68a8a0ffaf0c47d13b4181ea</t>
+  </si>
+  <si>
+    <t>9a47e4970377569015ef80b957a9e6c9</t>
+  </si>
+  <si>
+    <t>cabdbe29e207198ffca58832ca1e7c0d</t>
+  </si>
+  <si>
+    <t>e9ec4fa534e9d05a59424553bd4ffdf6</t>
+  </si>
+  <si>
+    <t>d1b24965eb3cfd018845da67fa1850bc</t>
+  </si>
+  <si>
+    <t>ac866f11b4d1ef3083d8769da6203a67</t>
+  </si>
+  <si>
+    <t>df0446869000b3a6b7b82a421a8e5273</t>
+  </si>
+  <si>
+    <t>1c078aa61a58baf35d57ceb5366e52fc</t>
+  </si>
+  <si>
+    <t>3b323211e3f52500005ee704d521cff4</t>
+  </si>
+  <si>
+    <t>0cfc3ee43c7964cbdad2237f0b68db64</t>
+  </si>
+  <si>
+    <t>ed6c1bb21e7fd960a37ceb39fbec6933</t>
+  </si>
+  <si>
+    <t>e2a26db2b8e08bcf7e2f81c5f7e2972c</t>
+  </si>
+  <si>
+    <t>49f4330718aba000f342fc250a3b4dbc</t>
+  </si>
+  <si>
+    <t>41c4951dac2c197bd4d5ed07ff59914e</t>
+  </si>
+  <si>
+    <t>f54b725a95775ff92b9f3d1e06829558</t>
+  </si>
+  <si>
+    <t>2bd49f0fdfe19878074e39e8c86b9789</t>
+  </si>
+  <si>
+    <t>318171f4834cf06049826225c22b9aa2</t>
+  </si>
+  <si>
+    <t>a9d2dc7e4792d06420644734e4b42630</t>
+  </si>
+  <si>
+    <t>82a2d3b363ed5c78101fdd96d8cd360a</t>
+  </si>
+  <si>
+    <t>ed866a931f11e7d19540321eab158507</t>
+  </si>
+  <si>
+    <t>a0cf5996f52d9fd7f9ef37a04a725196</t>
+  </si>
+  <si>
+    <t>f471246e7f946d08bd763fa512f56cd0</t>
+  </si>
+  <si>
+    <t>b913c39657ba36175b85b4e43343eb9b</t>
+  </si>
+  <si>
+    <t>8506cce1a9c4bf5ab5a8ef1630bc01ea</t>
+  </si>
+  <si>
+    <t>2978194f604c56db0c4c97814da135f7</t>
+  </si>
+  <si>
+    <t>65d51ae75ab896e1559e8a1ea9937bd1</t>
+  </si>
+  <si>
+    <t>e51c69ea4c87be44b0942490ba2bd643</t>
+  </si>
+  <si>
+    <t>f28a721fe50bbe88c90a76869aa6b1c4</t>
+  </si>
+  <si>
+    <t>4d4bbd575ccbfb50261abc8576378caa</t>
+  </si>
+  <si>
+    <t>7916a03e672fbe8e9c6551952c37a702</t>
+  </si>
+  <si>
+    <t>fa5430f711b88ec1de82a3263faea716</t>
+  </si>
+  <si>
+    <t>0991a0d7d509cc9bb61eb241fdc98798</t>
+  </si>
+  <si>
+    <t>955647fea0b807e75ac16a2b1140adf3</t>
+  </si>
+  <si>
+    <t>d80781d60a135d10479589a434640c08</t>
+  </si>
+  <si>
+    <t>9ee99e92c1277e5020faa4abed2d0699</t>
+  </si>
+  <si>
+    <t>30f67c479152c841478b53718b9cb305</t>
+  </si>
+  <si>
+    <t>c5b5921d79a97b670562f47fe395677d</t>
+  </si>
+  <si>
+    <t>34b7bf3eef1f958258deb92846cfcbb3</t>
+  </si>
+  <si>
+    <t>3931552e9f9f68a7bd42a87aa6538ce3</t>
+  </si>
+  <si>
+    <t>c988129eec03c2cc4d047bb610347f24</t>
+  </si>
+  <si>
+    <t>e30a85a3f83d4ee1b87d16fb23897556</t>
+  </si>
+  <si>
+    <t>592f0b9322373b09995f66291928b1f0</t>
+  </si>
+  <si>
+    <t>7febe95bea2f13b95a0bfa370c692d0c</t>
+  </si>
+  <si>
+    <t>a8bbf5740c6e14d1e77e62a16b44e135</t>
+  </si>
+  <si>
+    <t>f53576a0f5f399716c5c8514371b0d59</t>
+  </si>
+  <si>
+    <t>a7057c9bdb2f5bbc70b817dcd445f5bb</t>
   </si>
 </sst>
 </file>
@@ -2100,13 +2238,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2931,47 +3081,47 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2999,6 +3149,10 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -3412,10 +3566,10 @@
   <dimension ref="A1:CL43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AX2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AZ42" sqref="AZ42"/>
+      <selection pane="bottomRight" activeCell="BB37" sqref="BB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3511,10 +3665,10 @@
       <c r="W1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="258" t="s">
+      <c r="X1" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="259"/>
+      <c r="Y1" s="253"/>
       <c r="Z1" s="250" t="s">
         <v>268</v>
       </c>
@@ -3931,7 +4085,7 @@
       <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="257" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="45">
@@ -4069,7 +4223,7 @@
       <c r="A5" s="34">
         <v>5</v>
       </c>
-      <c r="B5" s="256"/>
+      <c r="B5" s="258"/>
       <c r="C5" s="46">
         <v>2</v>
       </c>
@@ -4205,7 +4359,7 @@
       <c r="A6" s="34">
         <v>7</v>
       </c>
-      <c r="B6" s="257"/>
+      <c r="B6" s="259"/>
       <c r="C6" s="46">
         <v>3</v>
       </c>
@@ -4341,7 +4495,7 @@
       <c r="A7" s="34">
         <v>9</v>
       </c>
-      <c r="B7" s="251"/>
+      <c r="B7" s="260"/>
       <c r="C7" s="46">
         <v>4</v>
       </c>
@@ -4477,7 +4631,7 @@
       <c r="A8" s="34">
         <v>11</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="261"/>
       <c r="C8" s="46">
         <v>5</v>
       </c>
@@ -4613,7 +4767,7 @@
       <c r="A9" s="34">
         <v>13</v>
       </c>
-      <c r="B9" s="252"/>
+      <c r="B9" s="261"/>
       <c r="C9" s="46">
         <v>6</v>
       </c>
@@ -4749,7 +4903,7 @@
       <c r="A10" s="34">
         <v>15</v>
       </c>
-      <c r="B10" s="252"/>
+      <c r="B10" s="261"/>
       <c r="C10" s="46">
         <v>7</v>
       </c>
@@ -4885,7 +5039,7 @@
       <c r="A11" s="35">
         <v>17</v>
       </c>
-      <c r="B11" s="254"/>
+      <c r="B11" s="263"/>
       <c r="C11" s="47">
         <v>8</v>
       </c>
@@ -5021,7 +5175,7 @@
       <c r="A12" s="33">
         <v>19</v>
       </c>
-      <c r="B12" s="260" t="s">
+      <c r="B12" s="254" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="204">
@@ -5174,14 +5328,18 @@
       <c r="BA12" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB12" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC12" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="223"/>
-      <c r="BE12" s="223"/>
+      <c r="BB12" s="251">
+        <v>26132363</v>
+      </c>
+      <c r="BC12" s="251">
+        <v>26132363</v>
+      </c>
+      <c r="BD12" s="223" t="s">
+        <v>281</v>
+      </c>
+      <c r="BE12" s="223" t="s">
+        <v>304</v>
+      </c>
       <c r="BF12" s="224" t="s">
         <v>217</v>
       </c>
@@ -5286,7 +5444,7 @@
       <c r="A13" s="34">
         <v>21</v>
       </c>
-      <c r="B13" s="261"/>
+      <c r="B13" s="255"/>
       <c r="C13" s="205">
         <v>2</v>
       </c>
@@ -5437,14 +5595,18 @@
       <c r="BA13" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB13" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD13" s="223"/>
-      <c r="BE13" s="223"/>
+      <c r="BB13" s="251">
+        <v>32776170</v>
+      </c>
+      <c r="BC13" s="251">
+        <v>32776170</v>
+      </c>
+      <c r="BD13" s="223" t="s">
+        <v>282</v>
+      </c>
+      <c r="BE13" s="223" t="s">
+        <v>305</v>
+      </c>
       <c r="BF13" s="224" t="s">
         <v>217</v>
       </c>
@@ -5549,7 +5711,7 @@
       <c r="A14" s="34">
         <v>23</v>
       </c>
-      <c r="B14" s="262"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="205">
         <v>3</v>
       </c>
@@ -5698,14 +5860,18 @@
       <c r="BA14" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB14" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC14" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD14" s="223"/>
-      <c r="BE14" s="223"/>
+      <c r="BB14" s="251">
+        <v>15374445</v>
+      </c>
+      <c r="BC14" s="251">
+        <v>15374445</v>
+      </c>
+      <c r="BD14" s="223" t="s">
+        <v>283</v>
+      </c>
+      <c r="BE14" s="223" t="s">
+        <v>306</v>
+      </c>
       <c r="BF14" s="224" t="s">
         <v>217</v>
       </c>
@@ -5810,7 +5976,7 @@
       <c r="A15" s="34">
         <v>25</v>
       </c>
-      <c r="B15" s="251"/>
+      <c r="B15" s="260"/>
       <c r="C15" s="205">
         <v>4</v>
       </c>
@@ -5961,14 +6127,18 @@
       <c r="BA15" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB15" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD15" s="223"/>
-      <c r="BE15" s="223"/>
+      <c r="BB15" s="251">
+        <v>20236324</v>
+      </c>
+      <c r="BC15" s="251">
+        <v>20236324</v>
+      </c>
+      <c r="BD15" s="223" t="s">
+        <v>284</v>
+      </c>
+      <c r="BE15" s="223" t="s">
+        <v>307</v>
+      </c>
       <c r="BF15" s="224" t="s">
         <v>217</v>
       </c>
@@ -6073,7 +6243,7 @@
       <c r="A16" s="34">
         <v>27</v>
       </c>
-      <c r="B16" s="252"/>
+      <c r="B16" s="261"/>
       <c r="C16" s="205">
         <v>5</v>
       </c>
@@ -6224,14 +6394,18 @@
       <c r="BA16" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB16" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC16" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD16" s="223"/>
-      <c r="BE16" s="223"/>
+      <c r="BB16" s="251">
+        <v>23475092</v>
+      </c>
+      <c r="BC16" s="251">
+        <v>23475092</v>
+      </c>
+      <c r="BD16" s="223" t="s">
+        <v>285</v>
+      </c>
+      <c r="BE16" s="223" t="s">
+        <v>308</v>
+      </c>
       <c r="BF16" s="224" t="s">
         <v>217</v>
       </c>
@@ -6336,7 +6510,7 @@
       <c r="A17" s="34">
         <v>29</v>
       </c>
-      <c r="B17" s="252"/>
+      <c r="B17" s="261"/>
       <c r="C17" s="205">
         <v>6</v>
       </c>
@@ -6487,14 +6661,18 @@
       <c r="BA17" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB17" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC17" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD17" s="223"/>
-      <c r="BE17" s="223"/>
+      <c r="BB17" s="251">
+        <v>19019111</v>
+      </c>
+      <c r="BC17" s="251">
+        <v>19019111</v>
+      </c>
+      <c r="BD17" s="223" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE17" s="223" t="s">
+        <v>309</v>
+      </c>
       <c r="BF17" s="224" t="s">
         <v>217</v>
       </c>
@@ -6599,7 +6777,7 @@
       <c r="A18" s="34">
         <v>31</v>
       </c>
-      <c r="B18" s="252"/>
+      <c r="B18" s="261"/>
       <c r="C18" s="205">
         <v>7</v>
       </c>
@@ -6750,14 +6928,18 @@
       <c r="BA18" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB18" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC18" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD18" s="223"/>
-      <c r="BE18" s="223"/>
+      <c r="BB18" s="251">
+        <v>23417974</v>
+      </c>
+      <c r="BC18" s="251">
+        <v>23417974</v>
+      </c>
+      <c r="BD18" s="223" t="s">
+        <v>287</v>
+      </c>
+      <c r="BE18" s="223" t="s">
+        <v>310</v>
+      </c>
       <c r="BF18" s="224" t="s">
         <v>217</v>
       </c>
@@ -6862,7 +7044,7 @@
       <c r="A19" s="35">
         <v>33</v>
       </c>
-      <c r="B19" s="254"/>
+      <c r="B19" s="263"/>
       <c r="C19" s="206">
         <v>8</v>
       </c>
@@ -7013,14 +7195,18 @@
       <c r="BA19" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB19" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC19" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD19" s="223"/>
-      <c r="BE19" s="223"/>
+      <c r="BB19" s="251">
+        <v>21959015</v>
+      </c>
+      <c r="BC19" s="251">
+        <v>21959015</v>
+      </c>
+      <c r="BD19" s="223" t="s">
+        <v>288</v>
+      </c>
+      <c r="BE19" s="223" t="s">
+        <v>311</v>
+      </c>
       <c r="BF19" s="224" t="s">
         <v>217</v>
       </c>
@@ -7125,7 +7311,7 @@
       <c r="A20" s="33">
         <v>35</v>
       </c>
-      <c r="B20" s="255" t="s">
+      <c r="B20" s="257" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="204">
@@ -7278,14 +7464,18 @@
       <c r="BA20" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB20" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD20" s="223"/>
-      <c r="BE20" s="223"/>
+      <c r="BB20" s="251">
+        <v>19349699</v>
+      </c>
+      <c r="BC20" s="251">
+        <v>19349699</v>
+      </c>
+      <c r="BD20" s="223" t="s">
+        <v>289</v>
+      </c>
+      <c r="BE20" s="223" t="s">
+        <v>312</v>
+      </c>
       <c r="BF20" s="224" t="s">
         <v>217</v>
       </c>
@@ -7390,7 +7580,7 @@
       <c r="A21" s="34">
         <v>37</v>
       </c>
-      <c r="B21" s="256"/>
+      <c r="B21" s="258"/>
       <c r="C21" s="207">
         <v>2</v>
       </c>
@@ -7541,14 +7731,18 @@
       <c r="BA21" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB21" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD21" s="223"/>
-      <c r="BE21" s="223"/>
+      <c r="BB21" s="251">
+        <v>24640452</v>
+      </c>
+      <c r="BC21" s="251">
+        <v>24640452</v>
+      </c>
+      <c r="BD21" s="223" t="s">
+        <v>290</v>
+      </c>
+      <c r="BE21" s="223" t="s">
+        <v>313</v>
+      </c>
       <c r="BF21" s="224" t="s">
         <v>217</v>
       </c>
@@ -7653,7 +7847,7 @@
       <c r="A22" s="34">
         <v>39</v>
       </c>
-      <c r="B22" s="257"/>
+      <c r="B22" s="259"/>
       <c r="C22" s="207">
         <v>3</v>
       </c>
@@ -7804,14 +7998,18 @@
       <c r="BA22" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB22" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC22" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD22" s="223"/>
-      <c r="BE22" s="223"/>
+      <c r="BB22" s="251">
+        <v>22292795</v>
+      </c>
+      <c r="BC22" s="251">
+        <v>22292795</v>
+      </c>
+      <c r="BD22" s="223" t="s">
+        <v>291</v>
+      </c>
+      <c r="BE22" s="223" t="s">
+        <v>314</v>
+      </c>
       <c r="BF22" s="224" t="s">
         <v>217</v>
       </c>
@@ -7916,7 +8114,7 @@
       <c r="A23" s="34">
         <v>41</v>
       </c>
-      <c r="B23" s="251"/>
+      <c r="B23" s="260"/>
       <c r="C23" s="205">
         <v>4</v>
       </c>
@@ -8067,14 +8265,18 @@
       <c r="BA23" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB23" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC23" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD23" s="223"/>
-      <c r="BE23" s="223"/>
+      <c r="BB23" s="251">
+        <v>24336672</v>
+      </c>
+      <c r="BC23" s="251">
+        <v>24336672</v>
+      </c>
+      <c r="BD23" s="223" t="s">
+        <v>292</v>
+      </c>
+      <c r="BE23" s="223" t="s">
+        <v>315</v>
+      </c>
       <c r="BF23" s="224" t="s">
         <v>217</v>
       </c>
@@ -8179,7 +8381,7 @@
       <c r="A24" s="34">
         <v>43</v>
       </c>
-      <c r="B24" s="252"/>
+      <c r="B24" s="261"/>
       <c r="C24" s="205">
         <v>5</v>
       </c>
@@ -8330,14 +8532,18 @@
       <c r="BA24" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB24" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC24" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD24" s="223"/>
-      <c r="BE24" s="223"/>
+      <c r="BB24" s="251">
+        <v>22153770</v>
+      </c>
+      <c r="BC24" s="251">
+        <v>22153770</v>
+      </c>
+      <c r="BD24" s="223" t="s">
+        <v>293</v>
+      </c>
+      <c r="BE24" s="223" t="s">
+        <v>316</v>
+      </c>
       <c r="BF24" s="224" t="s">
         <v>217</v>
       </c>
@@ -8442,7 +8648,7 @@
       <c r="A25" s="34">
         <v>45</v>
       </c>
-      <c r="B25" s="252"/>
+      <c r="B25" s="261"/>
       <c r="C25" s="205">
         <v>6</v>
       </c>
@@ -8593,14 +8799,18 @@
       <c r="BA25" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB25" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC25" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD25" s="223"/>
-      <c r="BE25" s="223"/>
+      <c r="BB25" s="251">
+        <v>23514431</v>
+      </c>
+      <c r="BC25" s="251">
+        <v>23514431</v>
+      </c>
+      <c r="BD25" s="223" t="s">
+        <v>294</v>
+      </c>
+      <c r="BE25" s="223" t="s">
+        <v>317</v>
+      </c>
       <c r="BF25" s="224" t="s">
         <v>217</v>
       </c>
@@ -8705,7 +8915,7 @@
       <c r="A26" s="34">
         <v>47</v>
       </c>
-      <c r="B26" s="252"/>
+      <c r="B26" s="261"/>
       <c r="C26" s="205">
         <v>7</v>
       </c>
@@ -8860,14 +9070,18 @@
       <c r="BA26" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB26" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC26" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD26" s="223"/>
-      <c r="BE26" s="223"/>
+      <c r="BB26" s="251">
+        <v>25239007</v>
+      </c>
+      <c r="BC26" s="251">
+        <v>25239007</v>
+      </c>
+      <c r="BD26" s="223" t="s">
+        <v>295</v>
+      </c>
+      <c r="BE26" s="223" t="s">
+        <v>318</v>
+      </c>
       <c r="BF26" s="224" t="s">
         <v>217</v>
       </c>
@@ -8972,7 +9186,7 @@
       <c r="A27" s="35">
         <v>49</v>
       </c>
-      <c r="B27" s="254"/>
+      <c r="B27" s="263"/>
       <c r="C27" s="206">
         <v>8</v>
       </c>
@@ -9127,14 +9341,18 @@
       <c r="BA27" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB27" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC27" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD27" s="223"/>
-      <c r="BE27" s="223"/>
+      <c r="BB27" s="251">
+        <v>26888537</v>
+      </c>
+      <c r="BC27" s="251">
+        <v>26888537</v>
+      </c>
+      <c r="BD27" s="223" t="s">
+        <v>296</v>
+      </c>
+      <c r="BE27" s="223" t="s">
+        <v>319</v>
+      </c>
       <c r="BF27" s="224" t="s">
         <v>217</v>
       </c>
@@ -9239,7 +9457,7 @@
       <c r="A28" s="33">
         <v>51</v>
       </c>
-      <c r="B28" s="255" t="s">
+      <c r="B28" s="257" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="204">
@@ -9390,14 +9608,18 @@
       <c r="BA28" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB28" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC28" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD28" s="223"/>
-      <c r="BE28" s="223"/>
+      <c r="BB28" s="251">
+        <v>24099741</v>
+      </c>
+      <c r="BC28" s="251">
+        <v>24099741</v>
+      </c>
+      <c r="BD28" s="223" t="s">
+        <v>297</v>
+      </c>
+      <c r="BE28" s="223" t="s">
+        <v>320</v>
+      </c>
       <c r="BF28" s="224" t="s">
         <v>217</v>
       </c>
@@ -9502,7 +9724,7 @@
       <c r="A29" s="34">
         <v>53</v>
       </c>
-      <c r="B29" s="256"/>
+      <c r="B29" s="258"/>
       <c r="C29" s="205">
         <v>2</v>
       </c>
@@ -9651,14 +9873,18 @@
       <c r="BA29" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB29" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC29" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD29" s="223"/>
-      <c r="BE29" s="223"/>
+      <c r="BB29" s="251">
+        <v>25131709</v>
+      </c>
+      <c r="BC29" s="251">
+        <v>25131709</v>
+      </c>
+      <c r="BD29" s="223" t="s">
+        <v>298</v>
+      </c>
+      <c r="BE29" s="223" t="s">
+        <v>321</v>
+      </c>
       <c r="BF29" s="224" t="s">
         <v>217</v>
       </c>
@@ -9763,7 +9989,7 @@
       <c r="A30" s="34">
         <v>55</v>
       </c>
-      <c r="B30" s="257"/>
+      <c r="B30" s="259"/>
       <c r="C30" s="205">
         <v>3</v>
       </c>
@@ -9912,14 +10138,18 @@
       <c r="BA30" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB30" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC30" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD30" s="223"/>
-      <c r="BE30" s="223"/>
+      <c r="BB30" s="251">
+        <v>25333059</v>
+      </c>
+      <c r="BC30" s="251">
+        <v>25333059</v>
+      </c>
+      <c r="BD30" s="223" t="s">
+        <v>299</v>
+      </c>
+      <c r="BE30" s="223" t="s">
+        <v>322</v>
+      </c>
       <c r="BF30" s="224" t="s">
         <v>217</v>
       </c>
@@ -10024,7 +10254,7 @@
       <c r="A31" s="34">
         <v>57</v>
       </c>
-      <c r="B31" s="251"/>
+      <c r="B31" s="260"/>
       <c r="C31" s="205">
         <v>4</v>
       </c>
@@ -10173,14 +10403,18 @@
       <c r="BA31" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB31" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC31" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD31" s="223"/>
-      <c r="BE31" s="223"/>
+      <c r="BB31" s="251">
+        <v>23643065</v>
+      </c>
+      <c r="BC31" s="251">
+        <v>23643065</v>
+      </c>
+      <c r="BD31" s="223" t="s">
+        <v>300</v>
+      </c>
+      <c r="BE31" s="223" t="s">
+        <v>323</v>
+      </c>
       <c r="BF31" s="224" t="s">
         <v>217</v>
       </c>
@@ -10285,7 +10519,7 @@
       <c r="A32" s="34">
         <v>59</v>
       </c>
-      <c r="B32" s="252"/>
+      <c r="B32" s="261"/>
       <c r="C32" s="205">
         <v>5</v>
       </c>
@@ -10434,14 +10668,18 @@
       <c r="BA32" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB32" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC32" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD32" s="223"/>
-      <c r="BE32" s="223"/>
+      <c r="BB32" s="251">
+        <v>23126069</v>
+      </c>
+      <c r="BC32" s="251">
+        <v>23126069</v>
+      </c>
+      <c r="BD32" s="223" t="s">
+        <v>301</v>
+      </c>
+      <c r="BE32" s="223" t="s">
+        <v>324</v>
+      </c>
       <c r="BF32" s="224" t="s">
         <v>217</v>
       </c>
@@ -10546,7 +10784,7 @@
       <c r="A33" s="34">
         <v>61</v>
       </c>
-      <c r="B33" s="252"/>
+      <c r="B33" s="261"/>
       <c r="C33" s="205">
         <v>6</v>
       </c>
@@ -10678,8 +10916,8 @@
       <c r="AV33" s="219"/>
       <c r="AZ33" s="223"/>
       <c r="BA33" s="223"/>
-      <c r="BB33" s="263"/>
-      <c r="BC33" s="263"/>
+      <c r="BB33" s="251"/>
+      <c r="BC33" s="251"/>
       <c r="BD33" s="223"/>
       <c r="BE33" s="223"/>
       <c r="BF33" s="224"/>
@@ -10713,7 +10951,7 @@
       <c r="A34" s="34">
         <v>63</v>
       </c>
-      <c r="B34" s="252"/>
+      <c r="B34" s="261"/>
       <c r="C34" s="205">
         <v>7</v>
       </c>
@@ -10862,14 +11100,18 @@
       <c r="BA34" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB34" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC34" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD34" s="223"/>
-      <c r="BE34" s="223"/>
+      <c r="BB34" s="251">
+        <v>21665592</v>
+      </c>
+      <c r="BC34" s="251">
+        <v>21665592</v>
+      </c>
+      <c r="BD34" s="223" t="s">
+        <v>302</v>
+      </c>
+      <c r="BE34" s="223" t="s">
+        <v>325</v>
+      </c>
       <c r="BF34" s="224" t="s">
         <v>217</v>
       </c>
@@ -10974,7 +11216,7 @@
       <c r="A35" s="35">
         <v>65</v>
       </c>
-      <c r="B35" s="254"/>
+      <c r="B35" s="263"/>
       <c r="C35" s="206">
         <v>8</v>
       </c>
@@ -11123,14 +11365,18 @@
       <c r="BA35" s="223" t="s">
         <v>273</v>
       </c>
-      <c r="BB35" s="263">
-        <v>0</v>
-      </c>
-      <c r="BC35" s="263">
-        <v>0</v>
-      </c>
-      <c r="BD35" s="223"/>
-      <c r="BE35" s="223"/>
+      <c r="BB35" s="251">
+        <v>24804911</v>
+      </c>
+      <c r="BC35" s="251">
+        <v>24804911</v>
+      </c>
+      <c r="BD35" s="223" t="s">
+        <v>303</v>
+      </c>
+      <c r="BE35" s="223" t="s">
+        <v>326</v>
+      </c>
       <c r="BF35" s="224" t="s">
         <v>217</v>
       </c>
@@ -11235,7 +11481,7 @@
       <c r="A36" s="33">
         <v>67</v>
       </c>
-      <c r="B36" s="255" t="s">
+      <c r="B36" s="257" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="45">
@@ -11373,7 +11619,7 @@
       <c r="A37" s="34">
         <v>69</v>
       </c>
-      <c r="B37" s="256"/>
+      <c r="B37" s="258"/>
       <c r="C37" s="46">
         <v>2</v>
       </c>
@@ -11509,7 +11755,7 @@
       <c r="A38" s="34">
         <v>71</v>
       </c>
-      <c r="B38" s="257"/>
+      <c r="B38" s="259"/>
       <c r="C38" s="46">
         <v>3</v>
       </c>
@@ -11645,7 +11891,7 @@
       <c r="A39" s="34">
         <v>73</v>
       </c>
-      <c r="B39" s="251"/>
+      <c r="B39" s="260"/>
       <c r="C39" s="46">
         <v>4</v>
       </c>
@@ -11779,7 +12025,7 @@
       <c r="A40" s="34">
         <v>75</v>
       </c>
-      <c r="B40" s="252"/>
+      <c r="B40" s="261"/>
       <c r="C40" s="46">
         <v>5</v>
       </c>
@@ -11919,7 +12165,7 @@
       <c r="A41" s="34">
         <v>77</v>
       </c>
-      <c r="B41" s="252"/>
+      <c r="B41" s="261"/>
       <c r="C41" s="46">
         <v>6</v>
       </c>
@@ -12055,7 +12301,7 @@
       <c r="A42" s="34">
         <v>79</v>
       </c>
-      <c r="B42" s="253"/>
+      <c r="B42" s="262"/>
       <c r="C42" s="48">
         <v>7</v>
       </c>
@@ -12189,17 +12435,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B28:B30"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B36:B38"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="BB1:BC1">

</xml_diff>